<commit_message>
66177 - Excel Template changes for header and footer
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESFA\Source\Repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43635E38-66F6-43ED-AF20-FA7C5016047A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8DF9B6-FA30-477C-AE91-4D9DFE1D3191}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
   </bookViews>
@@ -365,7 +365,7 @@
       <xdr:row>60</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7651749" cy="3238500"/>
+    <xdr:ext cx="6343649" cy="4219574"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
@@ -379,8 +379,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="127001" y="11430001"/>
-          <a:ext cx="7651749" cy="3238500"/>
+          <a:off x="133351" y="11325226"/>
+          <a:ext cx="6343649" cy="4219574"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -556,7 +556,7 @@
       <xdr:row>98</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5543550" cy="7877175"/>
+    <xdr:ext cx="5105400" cy="8029575"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="TextBox 3">
@@ -570,8 +570,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="133350" y="17735550"/>
-          <a:ext cx="5543550" cy="7877175"/>
+          <a:off x="123825" y="17497425"/>
+          <a:ext cx="5105400" cy="8029575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1500,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B3A90E-3784-4013-A5C0-29D9C7CC6C84}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1522,9 +1522,9 @@
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -1543,9 +1543,7 @@
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1554,9 +1552,7 @@
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -2208,7 +2204,7 @@
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="D58:F58"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="1.25" bottom="1.25" header="0.1" footer="0.1"/>
+  <pageMargins left="0.3" right="0.3" top="1.25" bottom="1.25" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
69122-aspose exception and placing header and footer contents in the report body
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESFA\Source\Repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8DF9B6-FA30-477C-AE91-4D9DFE1D3191}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D6AF0-7450-4141-9128-F4651D7E88F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>Retention Factor (allocation)</t>
   </si>
@@ -136,6 +136,51 @@
   </si>
   <si>
     <t>£-</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>UKPRN</t>
+  </si>
+  <si>
+    <t>ILR File</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Reference Date</t>
+  </si>
+  <si>
+    <t>Campus Identifier</t>
+  </si>
+  <si>
+    <t>Component Set Version</t>
+  </si>
+  <si>
+    <t>Application Version</t>
+  </si>
+  <si>
+    <t>File Preparation Date</t>
+  </si>
+  <si>
+    <t>Lars Data</t>
+  </si>
+  <si>
+    <t>Organisation Data</t>
+  </si>
+  <si>
+    <t>Postcode Data</t>
+  </si>
+  <si>
+    <t>Large Employer Data</t>
+  </si>
+  <si>
+    <t>CoF Removal Data</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -146,7 +191,7 @@
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +223,28 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -289,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -325,6 +392,26 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -337,6 +424,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -362,7 +461,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6343649" cy="4219574"/>
@@ -551,12 +650,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123823</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5105400" cy="8029575"/>
+    <xdr:ext cx="8750302" cy="5873750"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="TextBox 3">
@@ -570,8 +669,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="123825" y="17497425"/>
-          <a:ext cx="5105400" cy="8029575"/>
+          <a:off x="123823" y="19510376"/>
+          <a:ext cx="8750302" cy="5873750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1498,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B3A90E-3784-4013-A5C0-29D9C7CC6C84}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152:F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1528,147 +1627,155 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="5"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="5"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="21"/>
+      <c r="B7" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>8</v>
-      </c>
+      <c r="B9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="B10" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="D14" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
@@ -1677,10 +1784,10 @@
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1689,190 +1796,194 @@
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="10">
-        <f>SUM(E10:E15)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="16">
-        <f>SUM(F10:F15)</f>
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E18" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>19</v>
-      </c>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E19" s="14"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="24"/>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="E20" s="10">
+        <f>SUM(E14:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="16">
+        <f>SUM(F14:F19)</f>
+        <v>0</v>
+      </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="24"/>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="E22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>19</v>
+      </c>
       <c r="D23" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="17"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="24"/>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="30"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="17"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
-      <c r="C25" s="25"/>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="10">
-        <f>SUM(E19:E24)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="16">
-        <f>SUM(F19:F24)</f>
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E27" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>21</v>
-      </c>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="30"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="30"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="30"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="17"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
-      <c r="C29" s="24"/>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="31"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="E29" s="10">
+        <f>SUM(E23:E28)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="16">
+        <f>SUM(F23:F28)</f>
+        <v>0</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="22"/>
-      <c r="C32" s="24"/>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="E31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="D32" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="17"/>
@@ -1880,10 +1991,10 @@
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="17"/>
@@ -1891,45 +2002,43 @@
       <c r="H33" s="15"/>
     </row>
     <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
-      <c r="C34" s="25"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="10">
-        <f>SUM(E28:E33)</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="16">
-        <f>SUM(F28:F33)</f>
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="17"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="30"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+    </row>
     <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E36" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="30"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="17"/>
@@ -1937,43 +2046,45 @@
       <c r="H37" s="15"/>
     </row>
     <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="22"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="33"/>
       <c r="D38" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="E38" s="10">
+        <f>SUM(E32:E37)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <f>SUM(F32:F37)</f>
+        <v>0</v>
+      </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-    </row>
     <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-    </row>
-    <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
-      <c r="C41" s="24"/>
+      <c r="E40" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>23</v>
+      </c>
       <c r="D41" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
@@ -1981,10 +2092,10 @@
       <c r="H41" s="15"/>
     </row>
     <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="22"/>
-      <c r="C42" s="24"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="17"/>
@@ -1992,63 +2103,76 @@
       <c r="H42" s="15"/>
     </row>
     <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-      <c r="C43" s="25"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="10">
-        <f>SUM(E37:E42)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="16">
-        <f>SUM(F37:F42)</f>
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="17"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
     </row>
+    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="30"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+    </row>
     <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="30"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="30"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="31"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="10">
-        <f>SUM(E16,E25,E34,E43)</f>
+      <c r="E47" s="10">
+        <f>SUM(E41:E46)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="11">
-        <f>SUM(F16,F25,F34,F43)</f>
+      <c r="F47" s="16">
+        <f>SUM(F41:F46)</f>
         <v>0</v>
       </c>
-      <c r="G45" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D47" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-    </row>
-    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="H48"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
     </row>
     <row r="49" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D49" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E49" s="10">
-        <f>SUM(E45,E47)</f>
+        <f>SUM(E20,E29,E38,E47)</f>
         <v>0</v>
       </c>
       <c r="F49" s="11">
-        <f>SUM(F45,F47)</f>
+        <f>SUM(F20,F29,F38,F47)</f>
         <v>0</v>
       </c>
       <c r="G49" s="11" t="s">
@@ -2058,153 +2182,270 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="H50" s="8"/>
+    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D51" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="19" t="s">
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D53" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="10">
+        <f>SUM(E49,E51)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="11">
+        <f>SUM(F49,F51)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H54" s="8"/>
+    </row>
+    <row r="56" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19" t="s">
+      <c r="C56" s="27"/>
+      <c r="D56" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="9" t="s">
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="19" t="s">
+    <row r="57" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19" t="s">
+      <c r="C57" s="27"/>
+      <c r="D57" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="9" t="s">
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="19" t="s">
+    <row r="58" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19" t="s">
+      <c r="C58" s="27"/>
+      <c r="D58" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="9" t="s">
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="19" t="s">
+    <row r="59" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19" t="s">
+      <c r="C59" s="27"/>
+      <c r="D59" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="9" t="s">
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
+    <row r="60" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
+      <c r="C60" s="27"/>
+      <c r="D60" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="9" t="s">
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
+    <row r="61" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19" t="s">
+      <c r="C61" s="27"/>
+      <c r="D61" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="9" t="s">
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="19" t="s">
+    <row r="62" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19" t="s">
+      <c r="C62" s="27"/>
+      <c r="D62" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="9" t="s">
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="2:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="108" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="2:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B152" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C152" s="23"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="22"/>
+      <c r="F152" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="G152" s="34"/>
+      <c r="H152" s="34"/>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B153" s="36"/>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="22"/>
+      <c r="F153" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G153" s="34"/>
+      <c r="H153" s="34"/>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B154" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C154" s="23"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="22"/>
+      <c r="F154" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="G154" s="34"/>
+      <c r="H154" s="34"/>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B155" s="36"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="22"/>
+      <c r="F155" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G155" s="34"/>
+      <c r="H155" s="34"/>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B156" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C156" s="23"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="22"/>
+      <c r="F156" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G156" s="34"/>
+      <c r="H156" s="34"/>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B157" s="36"/>
+      <c r="C157" s="24"/>
+      <c r="D157" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B10:B16"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="C19:C25"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:F55"/>
+  <mergeCells count="41">
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="C41:C47"/>
     <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:F62"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="D57:F57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="D58:F58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C29"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="C152:D153"/>
+    <mergeCell ref="C154:D155"/>
+    <mergeCell ref="C156:D157"/>
+    <mergeCell ref="G152:H152"/>
+    <mergeCell ref="G153:H153"/>
+    <mergeCell ref="G154:H154"/>
+    <mergeCell ref="G155:H155"/>
+    <mergeCell ref="G156:H156"/>
   </mergeCells>
-  <pageMargins left="0.3" right="0.3" top="1.25" bottom="1.25" header="0.1" footer="0.1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
70150, 70140, 70141, 70139, 70137 - various formatting issues with the report
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D6AF0-7450-4141-9128-F4651D7E88F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D48219-1582-4586-9F31-B6CCCC79F007}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
+    <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="2" r:id="rId1"/>
@@ -267,18 +267,9 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -351,91 +342,225 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -459,12 +584,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6343649" cy="4219574"/>
+    <xdr:ext cx="8334374" cy="3371849"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
@@ -478,8 +603,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="133351" y="11325226"/>
-          <a:ext cx="6343649" cy="4219574"/>
+          <a:off x="28576" y="14630401"/>
+          <a:ext cx="8334374" cy="3371849"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -651,11 +776,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123823</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:colOff>76198</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8750302" cy="5873750"/>
+    <xdr:ext cx="8229602" cy="6638925"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="TextBox 3">
@@ -669,8 +794,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="123823" y="19510376"/>
-          <a:ext cx="8750302" cy="5873750"/>
+          <a:off x="76198" y="19316700"/>
+          <a:ext cx="8229602" cy="6638925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1224,6 +1349,18 @@
             <a:rPr lang="en-US" sz="900"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:endParaRPr lang="en-US" sz="900"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:endParaRPr lang="en-US" sz="900"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:endParaRPr lang="en-US" sz="900"/>
         </a:p>
         <a:p>
           <a:pPr algn="just"/>
@@ -1597,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B3A90E-3784-4013-A5C0-29D9C7CC6C84}">
-  <dimension ref="A1:I157"/>
+  <dimension ref="B1:H158"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152:F156"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1611,842 +1748,886 @@
     <col min="4" max="4" width="24.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+    <row r="1" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="20" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="36"/>
+      <c r="G3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="19" t="s">
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="20" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="36"/>
+      <c r="G4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+    </row>
+    <row r="5" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="20" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="36"/>
+      <c r="G5" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="28" t="s">
+    </row>
+    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="28" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="28" t="s">
+      <c r="C9" s="40"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="28" t="s">
+      <c r="C10" s="40"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="14" t="s">
+      <c r="C11" s="40"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="30" t="s">
+    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="43" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="32"/>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="41"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="32"/>
+      <c r="E15" s="22">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="41"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="32"/>
+      <c r="E16" s="22">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="41"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="32"/>
+      <c r="E17" s="22">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="41"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="32"/>
+      <c r="E18" s="22">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="41"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="10" t="s">
+      <c r="E19" s="22">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="23">
         <f>SUM(E14:E19)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="12">
         <f>SUM(F14:F19)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E22" s="14" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="30"/>
-      <c r="C24" s="32"/>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="41"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
-      <c r="C25" s="32"/>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="41"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="30"/>
-      <c r="C26" s="32"/>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="41"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
-      <c r="C27" s="32"/>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="41"/>
+      <c r="C27" s="43"/>
       <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
-      <c r="C28" s="32"/>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="41"/>
+      <c r="C28" s="43"/>
       <c r="D28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="10" t="s">
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="42"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="6">
         <f>SUM(E23:E28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="12">
         <f>SUM(F23:F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E31" s="14" t="s">
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E32" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G32" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H32" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
+    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C33" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="30"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10">
+        <v>0</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="41"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="41"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="30"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10">
+        <v>0</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="41"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="10">
+        <v>0</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="41"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="14"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="10">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="41"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="31"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10">
+        <v>0</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="42"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="10">
-        <f>SUM(E32:E37)</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="16">
-        <f>SUM(F32:F37)</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-    </row>
-    <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E40" s="14" t="s">
+      <c r="E39" s="6">
+        <f>SUM(E33:E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="12">
+        <f>SUM(F33:F38)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="41" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G41" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H41" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="30" t="s">
+    <row r="42" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C42" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" s="41"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-    </row>
-    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="10" t="s">
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="41"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-    </row>
-    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10">
+        <v>0</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="41"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-    </row>
-    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="13"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="41"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="14"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="30"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="41"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="31"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="10" t="s">
+      <c r="E47" s="10">
+        <v>0</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" s="42"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="10">
-        <f>SUM(E41:E46)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="16">
-        <f>SUM(F41:F46)</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="49" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="D49" s="10" t="s">
+      <c r="E48" s="6">
+        <f>SUM(E42:E47)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="12">
+        <f>SUM(F42:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="50" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D50" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="10">
-        <f>SUM(E20,E29,E38,E47)</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="11">
-        <f>SUM(F20,F29,F38,F47)</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="11" t="s">
+      <c r="E50" s="6">
+        <f>SUM(E20,E29,E39,E48)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="7">
+        <f>SUM(F20,F29,F39,F48)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H50" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D51" s="12" t="s">
+    <row r="52" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D52" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-    </row>
-    <row r="52" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="H52"/>
-    </row>
-    <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="D53" s="10" t="s">
+      <c r="E52" s="9"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="10">
-        <f>SUM(E49,E51)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="11">
-        <f>SUM(F49,F51)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="11" t="s">
+      <c r="E54" s="6">
+        <f>SUM(E50,E52)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="7">
+        <f>SUM(F50,F52)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H54" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="H54" s="8"/>
-    </row>
-    <row r="56" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
+    <row r="55" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H55" s="4"/>
+    </row>
+    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B66" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27" t="s">
+      <c r="C66" s="45"/>
+      <c r="D66" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="9" t="s">
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
+    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B67" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27" t="s">
+      <c r="C67" s="45"/>
+      <c r="D67" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="9" t="s">
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
+    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B68" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27" t="s">
+      <c r="C68" s="45"/>
+      <c r="D68" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="9" t="s">
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="27" t="s">
+    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B69" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27" t="s">
+      <c r="C69" s="45"/>
+      <c r="D69" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="9" t="s">
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="27" t="s">
+    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B70" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27" t="s">
+      <c r="C70" s="45"/>
+      <c r="D70" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="9" t="s">
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="27" t="s">
+    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B71" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27" t="s">
+      <c r="C71" s="45"/>
+      <c r="D71" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="9" t="s">
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="27" t="s">
+    <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B72" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27" t="s">
+      <c r="C72" s="45"/>
+      <c r="D72" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="9" t="s">
+      <c r="E72" s="47"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-    </row>
-    <row r="108" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
-      <c r="H108" s="18"/>
-    </row>
-    <row r="109" spans="2:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+    </row>
+    <row r="103" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="104" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B149" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C149" s="51"/>
+      <c r="D149" s="48"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G149" s="31"/>
+      <c r="H149" s="32"/>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B150" s="50"/>
+      <c r="C150" s="48"/>
+      <c r="D150" s="48"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="53"/>
+      <c r="G150" s="33"/>
+      <c r="H150" s="34"/>
+    </row>
+    <row r="151" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B151" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C151" s="51"/>
+      <c r="D151" s="48"/>
+      <c r="E151" s="16"/>
+      <c r="F151" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="G151" s="27"/>
+      <c r="H151" s="28"/>
+    </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B152" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C152" s="23"/>
-      <c r="D152" s="24"/>
-      <c r="E152" s="22"/>
-      <c r="F152" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="G152" s="34"/>
-      <c r="H152" s="34"/>
+      <c r="B152" s="50"/>
+      <c r="C152" s="48"/>
+      <c r="D152" s="48"/>
+      <c r="E152" s="16"/>
+      <c r="F152" s="54"/>
+      <c r="G152" s="29"/>
+      <c r="H152" s="30"/>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B153" s="36"/>
-      <c r="C153" s="24"/>
-      <c r="D153" s="24"/>
-      <c r="E153" s="22"/>
-      <c r="F153" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G153" s="34"/>
-      <c r="H153" s="34"/>
-    </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B154" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C154" s="23"/>
-      <c r="D154" s="24"/>
-      <c r="E154" s="22"/>
-      <c r="F154" s="37" t="s">
+      <c r="B153" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C153" s="51"/>
+      <c r="D153" s="48"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G154" s="34"/>
+      <c r="G153" s="31"/>
+      <c r="H153" s="32"/>
+    </row>
+    <row r="154" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="50"/>
+      <c r="C154" s="48"/>
+      <c r="D154" s="48"/>
+      <c r="F154" s="53"/>
+      <c r="G154" s="33"/>
       <c r="H154" s="34"/>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B155" s="36"/>
-      <c r="C155" s="24"/>
-      <c r="D155" s="24"/>
-      <c r="E155" s="22"/>
-      <c r="F155" s="37" t="s">
+      <c r="F155" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G155" s="34"/>
-      <c r="H155" s="34"/>
-    </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B156" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C156" s="23"/>
-      <c r="D156" s="24"/>
-      <c r="E156" s="22"/>
-      <c r="F156" s="37" t="s">
+      <c r="G155" s="27"/>
+      <c r="H155" s="28"/>
+    </row>
+    <row r="156" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F156" s="53"/>
+      <c r="G156" s="29"/>
+      <c r="H156" s="30"/>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F157" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G156" s="34"/>
-      <c r="H156" s="34"/>
-    </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B157" s="36"/>
-      <c r="C157" s="24"/>
-      <c r="D157" s="24"/>
+      <c r="G157" s="27"/>
+      <c r="H157" s="28"/>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F158" s="53"/>
+      <c r="G158" s="29"/>
+      <c r="H158" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D56:F56"/>
+  <mergeCells count="51">
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="F155:F156"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="C149:D150"/>
+    <mergeCell ref="C151:D152"/>
+    <mergeCell ref="C153:D154"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C29"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="C23:C29"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="C152:D153"/>
-    <mergeCell ref="C154:D155"/>
-    <mergeCell ref="C156:D157"/>
-    <mergeCell ref="G152:H152"/>
-    <mergeCell ref="G153:H153"/>
-    <mergeCell ref="G154:H154"/>
-    <mergeCell ref="G155:H155"/>
-    <mergeCell ref="G156:H156"/>
+    <mergeCell ref="G157:H158"/>
+    <mergeCell ref="G155:H156"/>
+    <mergeCell ref="G151:H152"/>
+    <mergeCell ref="G149:H150"/>
+    <mergeCell ref="G153:H154"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
70368, 70642, 70643, 70620, 70137 - 16-19 Funding claim missing values and formats
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D48219-1582-4586-9F31-B6CCCC79F007}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFF3B36-383F-43CA-8789-11605F0F8F8D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>Retention Factor (allocation)</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>£0.00</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -465,7 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -491,6 +493,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -515,19 +520,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,6 +548,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -561,6 +569,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1736,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B3A90E-3784-4013-A5C0-29D9C7CC6C84}">
   <dimension ref="B1:H158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1754,96 +1769,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="36"/>
-      <c r="G3" s="25" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="35"/>
+      <c r="G3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="36"/>
-      <c r="G4" s="25" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="35"/>
+      <c r="G4" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="36"/>
-      <c r="G5" s="26" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="35"/>
+      <c r="G5" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-    </row>
-    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
@@ -1860,7 +1875,7 @@
       <c r="F13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H13" s="10" t="s">
@@ -1868,16 +1883,16 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="42" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <v>0</v>
       </c>
       <c r="F14" s="11"/>
@@ -1885,12 +1900,12 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="43"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>0</v>
       </c>
       <c r="F15" s="11"/>
@@ -1898,12 +1913,12 @@
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="43"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>0</v>
       </c>
       <c r="F16" s="11"/>
@@ -1911,12 +1926,12 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="43"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>0</v>
       </c>
       <c r="F17" s="11"/>
@@ -1924,12 +1939,12 @@
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>0</v>
       </c>
       <c r="F18" s="11"/>
@@ -1937,12 +1952,12 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <v>0</v>
       </c>
       <c r="F19" s="11"/>
@@ -1950,12 +1965,12 @@
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="44"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <f>SUM(E14:E19)</f>
         <v>0</v>
       </c>
@@ -1973,7 +1988,7 @@
       <c r="F22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="10" t="s">
@@ -1981,10 +1996,10 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="42" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -1993,78 +2008,90 @@
       <c r="E23" s="10">
         <v>0</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="10">
         <v>0</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
-      <c r="C25" s="43"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="10">
         <v>0</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="41"/>
-      <c r="C26" s="43"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="13"/>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="43"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="41"/>
-      <c r="C28" s="43"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="10">
         <v>0</v>
       </c>
-      <c r="F28" s="13"/>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
     </row>
     <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="42"/>
-      <c r="C29" s="44"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="6" t="s">
         <v>17</v>
       </c>
@@ -2081,12 +2108,12 @@
     </row>
     <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B30"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="E32" s="10" t="s">
@@ -2095,7 +2122,7 @@
       <c r="F32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H32" s="10" t="s">
@@ -2103,10 +2130,10 @@
       </c>
     </row>
     <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="42" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -2115,77 +2142,89 @@
       <c r="E33" s="10">
         <v>0</v>
       </c>
-      <c r="F33" s="13"/>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="43"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="10">
         <v>0</v>
       </c>
-      <c r="F34" s="13"/>
+      <c r="F34" s="10">
+        <v>0</v>
+      </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
     </row>
     <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="41"/>
-      <c r="C35" s="43"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E35" s="10">
         <v>0</v>
       </c>
-      <c r="F35" s="13"/>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
     <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="41"/>
-      <c r="C36" s="43"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="10">
         <v>0</v>
       </c>
-      <c r="F36" s="13"/>
+      <c r="F36" s="10">
+        <v>0</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="41"/>
-      <c r="C37" s="43"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E37" s="10">
         <v>0</v>
       </c>
-      <c r="F37" s="13"/>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
     <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="41"/>
-      <c r="C38" s="43"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="10">
         <v>0</v>
       </c>
-      <c r="F38" s="13"/>
+      <c r="F38" s="10">
+        <v>0</v>
+      </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="42"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="48"/>
       <c r="D39" s="6" t="s">
         <v>17</v>
@@ -2208,7 +2247,7 @@
       <c r="F41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H41" s="10" t="s">
@@ -2216,10 +2255,10 @@
       </c>
     </row>
     <row r="42" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -2228,78 +2267,90 @@
       <c r="E42" s="10">
         <v>0</v>
       </c>
-      <c r="F42" s="13"/>
+      <c r="F42" s="10">
+        <v>0</v>
+      </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
     <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="41"/>
-      <c r="C43" s="43"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="42"/>
       <c r="D43" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="10">
         <v>0</v>
       </c>
-      <c r="F43" s="13"/>
+      <c r="F43" s="10">
+        <v>0</v>
+      </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
     </row>
     <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="41"/>
-      <c r="C44" s="43"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="42"/>
       <c r="D44" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="10">
         <v>0</v>
       </c>
-      <c r="F44" s="13"/>
+      <c r="F44" s="10">
+        <v>0</v>
+      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
     <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="41"/>
-      <c r="C45" s="43"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="42"/>
       <c r="D45" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E45" s="10">
         <v>0</v>
       </c>
-      <c r="F45" s="13"/>
+      <c r="F45" s="10">
+        <v>0</v>
+      </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
     <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="41"/>
-      <c r="C46" s="43"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="42"/>
       <c r="D46" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="10">
         <v>0</v>
       </c>
-      <c r="F46" s="13"/>
+      <c r="F46" s="10">
+        <v>0</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
     <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="41"/>
-      <c r="C47" s="43"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="10">
         <v>0</v>
       </c>
-      <c r="F47" s="13"/>
+      <c r="F47" s="10">
+        <v>0</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
     <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="42"/>
-      <c r="C48" s="44"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="43"/>
       <c r="D48" s="6" t="s">
         <v>17</v>
       </c>
@@ -2338,7 +2389,9 @@
         <v>24</v>
       </c>
       <c r="E52" s="9"/>
-      <c r="F52" s="6"/>
+      <c r="F52" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
@@ -2368,118 +2421,118 @@
       <c r="H55" s="4"/>
     </row>
     <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="45"/>
-      <c r="D66" s="46" t="s">
+      <c r="C66" s="44"/>
+      <c r="D66" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="36"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="47"/>
       <c r="H66" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="45" t="s">
+      <c r="B67" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="45"/>
-      <c r="D67" s="46" t="s">
+      <c r="C67" s="44"/>
+      <c r="D67" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="36"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="47"/>
       <c r="H67" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="45"/>
-      <c r="D68" s="46" t="s">
+      <c r="C68" s="44"/>
+      <c r="D68" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="36"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="47"/>
       <c r="H68" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46" t="s">
+      <c r="C69" s="44"/>
+      <c r="D69" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="36"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="47"/>
       <c r="H69" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="45" t="s">
+      <c r="B70" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="45"/>
-      <c r="D70" s="46" t="s">
+      <c r="C70" s="44"/>
+      <c r="D70" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="36"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="47"/>
       <c r="H70" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="45" t="s">
+      <c r="B71" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C71" s="45"/>
-      <c r="D71" s="46" t="s">
+      <c r="C71" s="44"/>
+      <c r="D71" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="36"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="47"/>
       <c r="H71" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="45" t="s">
+      <c r="B72" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="46" t="s">
+      <c r="C72" s="44"/>
+      <c r="D72" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="36"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="47"/>
       <c r="H72" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="102" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="14"/>
-      <c r="H102" s="14"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
     </row>
     <row r="103" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="104" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -2489,7 +2542,7 @@
       </c>
       <c r="C149" s="51"/>
       <c r="D149" s="48"/>
-      <c r="E149" s="16"/>
+      <c r="E149" s="15"/>
       <c r="F149" s="52" t="s">
         <v>46</v>
       </c>
@@ -2500,7 +2553,7 @@
       <c r="B150" s="50"/>
       <c r="C150" s="48"/>
       <c r="D150" s="48"/>
-      <c r="E150" s="16"/>
+      <c r="E150" s="15"/>
       <c r="F150" s="53"/>
       <c r="G150" s="33"/>
       <c r="H150" s="34"/>
@@ -2511,7 +2564,7 @@
       </c>
       <c r="C151" s="51"/>
       <c r="D151" s="48"/>
-      <c r="E151" s="16"/>
+      <c r="E151" s="15"/>
       <c r="F151" s="52" t="s">
         <v>47</v>
       </c>
@@ -2522,7 +2575,7 @@
       <c r="B152" s="50"/>
       <c r="C152" s="48"/>
       <c r="D152" s="48"/>
-      <c r="E152" s="16"/>
+      <c r="E152" s="15"/>
       <c r="F152" s="54"/>
       <c r="G152" s="29"/>
       <c r="H152" s="30"/>
@@ -2533,7 +2586,7 @@
       </c>
       <c r="C153" s="51"/>
       <c r="D153" s="48"/>
-      <c r="E153" s="16"/>
+      <c r="E153" s="15"/>
       <c r="F153" s="52" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
70643-CoFRemoval value; excel template change; unit tests
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Service/Reports/Templates/1619FundingClaimReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR1819.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D0579E-EF1B-4DCC-82DC-97316C4CDA46}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EEE5A8-3459-4346-9099-0E3F167F96FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42C50C4E-9E61-4A7D-9E12-F846D541E53C}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>Retention Factor (allocation)</t>
   </si>
@@ -181,18 +181,16 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>£0.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -444,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -483,7 +481,6 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -493,29 +490,55 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,59 +554,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7C274CC1-D68C-4D38-B979-3C42BC22AC14}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -1762,24 +1777,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B3A90E-3784-4013-A5C0-29D9C7CC6C84}">
   <dimension ref="B1:H158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="1.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.86328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1788,96 +1803,96 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+    <row r="2" spans="2:8" ht="13.15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="G3" s="24" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="G3" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="G4" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="2:8" ht="26.25" x14ac:dyDescent="0.35">
+      <c r="B5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
-      <c r="G5" s="25" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
+      <c r="G5" s="24" t="s">
         <v>42</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="47" t="s">
+    <row r="7" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B7" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B8" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
-    </row>
-    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="47" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B9" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="47" t="s">
+    <row r="10" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="47" t="s">
+    <row r="11" spans="2:8" ht="14.25" x14ac:dyDescent="0.35">
+      <c r="B11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="13.15" x14ac:dyDescent="0.35">
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C13"/>
       <c r="D13" s="2"/>
       <c r="E13" s="10" t="s">
@@ -1893,11 +1908,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B14" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1910,9 +1925,9 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="36"/>
+    <row r="15" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B15" s="44"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
@@ -1923,9 +1938,9 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="36"/>
+    <row r="16" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B16" s="44"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
@@ -1936,9 +1951,9 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="36"/>
+    <row r="17" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B17" s="44"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1949,9 +1964,9 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="36"/>
+    <row r="18" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B18" s="44"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
@@ -1962,9 +1977,9 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="36"/>
+    <row r="19" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B19" s="44"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="10" t="s">
         <v>16</v>
       </c>
@@ -1975,13 +1990,13 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="37"/>
+    <row r="20" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B20" s="45"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <f>SUM(E14:E19)</f>
         <v>0</v>
       </c>
@@ -1992,7 +2007,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E22" s="10" t="s">
         <v>5</v>
       </c>
@@ -2006,11 +2021,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34" t="s">
+    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -2019,90 +2034,90 @@
       <c r="E23" s="10">
         <v>0</v>
       </c>
-      <c r="F23" s="57">
+      <c r="F23" s="25">
         <v>0</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="36"/>
+    <row r="24" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B24" s="44"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="10">
         <v>0</v>
       </c>
-      <c r="F24" s="57">
+      <c r="F24" s="25">
         <v>0</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
-      <c r="C25" s="36"/>
+    <row r="25" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="10">
         <v>0</v>
       </c>
-      <c r="F25" s="57">
+      <c r="F25" s="25">
         <v>0</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="34"/>
-      <c r="C26" s="36"/>
+    <row r="26" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B26" s="44"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="57">
+      <c r="F26" s="25">
         <v>0</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="34"/>
-      <c r="C27" s="36"/>
+    <row r="27" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B27" s="44"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="10">
         <v>0</v>
       </c>
-      <c r="F27" s="57">
+      <c r="F27" s="25">
         <v>0</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="36"/>
+    <row r="28" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B28" s="44"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="10">
         <v>0</v>
       </c>
-      <c r="F28" s="57">
+      <c r="F28" s="25">
         <v>0</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
-      <c r="C29" s="37"/>
+    <row r="29" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B29" s="45"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="6" t="s">
         <v>17</v>
       </c>
@@ -2117,7 +2132,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B30"/>
       <c r="C30" s="16"/>
       <c r="D30" s="18"/>
@@ -2126,7 +2141,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
     </row>
-    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E32" s="10" t="s">
         <v>5</v>
       </c>
@@ -2140,11 +2155,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
+    <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -2153,90 +2168,90 @@
       <c r="E33" s="10">
         <v>0</v>
       </c>
-      <c r="F33" s="57">
+      <c r="F33" s="25">
         <v>0</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="34"/>
-      <c r="C34" s="36"/>
+    <row r="34" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B34" s="44"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="10">
         <v>0</v>
       </c>
-      <c r="F34" s="57">
+      <c r="F34" s="25">
         <v>0</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
-      <c r="C35" s="36"/>
+    <row r="35" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B35" s="44"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E35" s="10">
         <v>0</v>
       </c>
-      <c r="F35" s="57">
+      <c r="F35" s="25">
         <v>0</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
-      <c r="C36" s="36"/>
+    <row r="36" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B36" s="44"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="10">
         <v>0</v>
       </c>
-      <c r="F36" s="57">
+      <c r="F36" s="25">
         <v>0</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="34"/>
-      <c r="C37" s="36"/>
+    <row r="37" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B37" s="44"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E37" s="10">
         <v>0</v>
       </c>
-      <c r="F37" s="57">
+      <c r="F37" s="25">
         <v>0</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="36"/>
+    <row r="38" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B38" s="44"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="10">
         <v>0</v>
       </c>
-      <c r="F38" s="57">
+      <c r="F38" s="25">
         <v>0</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="35"/>
-      <c r="C39" s="33"/>
+    <row r="39" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B39" s="45"/>
+      <c r="C39" s="52"/>
       <c r="D39" s="6" t="s">
         <v>17</v>
       </c>
@@ -2251,7 +2266,7 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="41" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E41" s="10" t="s">
         <v>5</v>
       </c>
@@ -2265,11 +2280,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="34" t="s">
+    <row r="42" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="46" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -2278,90 +2293,90 @@
       <c r="E42" s="10">
         <v>0</v>
       </c>
-      <c r="F42" s="57">
+      <c r="F42" s="25">
         <v>0</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
-    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="34"/>
-      <c r="C43" s="36"/>
+    <row r="43" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B43" s="44"/>
+      <c r="C43" s="46"/>
       <c r="D43" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="10">
         <v>0</v>
       </c>
-      <c r="F43" s="57">
+      <c r="F43" s="25">
         <v>0</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
-      <c r="C44" s="36"/>
+    <row r="44" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B44" s="44"/>
+      <c r="C44" s="46"/>
       <c r="D44" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="10">
         <v>0</v>
       </c>
-      <c r="F44" s="57">
+      <c r="F44" s="25">
         <v>0</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="34"/>
-      <c r="C45" s="36"/>
+    <row r="45" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B45" s="44"/>
+      <c r="C45" s="46"/>
       <c r="D45" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E45" s="10">
         <v>0</v>
       </c>
-      <c r="F45" s="57">
+      <c r="F45" s="25">
         <v>0</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
-    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="34"/>
-      <c r="C46" s="36"/>
+    <row r="46" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B46" s="44"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="10">
         <v>0</v>
       </c>
-      <c r="F46" s="57">
+      <c r="F46" s="25">
         <v>0</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="34"/>
-      <c r="C47" s="36"/>
+    <row r="47" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B47" s="44"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="10">
         <v>0</v>
       </c>
-      <c r="F47" s="57">
+      <c r="F47" s="25">
         <v>0</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
-    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="35"/>
-      <c r="C48" s="37"/>
+    <row r="48" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B48" s="45"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="6" t="s">
         <v>17</v>
       </c>
@@ -2376,15 +2391,15 @@
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
-    <row r="50" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="D50" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="26">
         <f>SUM(E20,E29,E39,E48)</f>
         <v>0</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="27">
         <f>SUM(F20,F29,F39,F48)</f>
         <v>0</v>
       </c>
@@ -2395,30 +2410,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D52" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="9"/>
-      <c r="F52" s="26" t="s">
-        <v>52</v>
-      </c>
+      <c r="F52" s="28"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="H53"/>
     </row>
-    <row r="54" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="D54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="6">
-        <f>SUM(E50,E52)</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="7">
-        <f>SUM(F50,F52)</f>
+      <c r="E54" s="26">
+        <f>E50+E52</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="27">
+        <f>F50+F52</f>
         <v>0</v>
       </c>
       <c r="G54" s="7" t="s">
@@ -2428,115 +2441,115 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="H55" s="4"/>
     </row>
-    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="38" t="s">
+    <row r="66" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B66" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="39" t="s">
+      <c r="C66" s="48"/>
+      <c r="D66" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="41"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="51"/>
       <c r="H66" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="38" t="s">
+    <row r="67" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B67" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="38"/>
-      <c r="D67" s="39" t="s">
+      <c r="C67" s="48"/>
+      <c r="D67" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="41"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="51"/>
       <c r="H67" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="38" t="s">
+    <row r="68" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B68" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="38"/>
-      <c r="D68" s="39" t="s">
+      <c r="C68" s="48"/>
+      <c r="D68" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="41"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="51"/>
       <c r="H68" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="38" t="s">
+    <row r="69" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B69" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="38"/>
-      <c r="D69" s="39" t="s">
+      <c r="C69" s="48"/>
+      <c r="D69" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="41"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="51"/>
       <c r="H69" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="38" t="s">
+    <row r="70" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B70" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="38"/>
-      <c r="D70" s="39" t="s">
+      <c r="C70" s="48"/>
+      <c r="D70" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="41"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="51"/>
       <c r="H70" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="38" t="s">
+    <row r="71" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B71" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C71" s="38"/>
-      <c r="D71" s="39" t="s">
+      <c r="C71" s="48"/>
+      <c r="D71" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E71" s="40"/>
-      <c r="F71" s="40"/>
-      <c r="G71" s="41"/>
+      <c r="E71" s="50"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="51"/>
       <c r="H71" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="38" t="s">
+    <row r="72" spans="2:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B72" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="39" t="s">
+      <c r="C72" s="48"/>
+      <c r="D72" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="E72" s="40"/>
-      <c r="F72" s="40"/>
-      <c r="G72" s="41"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="51"/>
       <c r="H72" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
       <c r="D102" s="13"/>
@@ -2545,104 +2558,132 @@
       <c r="G102" s="13"/>
       <c r="H102" s="13"/>
     </row>
-    <row r="103" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="104" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B149" s="30" t="s">
+    <row r="103" spans="2:8" ht="13.15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="104" spans="2:8" ht="13.15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="149" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B149" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C149" s="32"/>
-      <c r="D149" s="33"/>
+      <c r="C149" s="55"/>
+      <c r="D149" s="52"/>
       <c r="E149" s="15"/>
-      <c r="F149" s="27" t="s">
+      <c r="F149" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="G149" s="53"/>
-      <c r="H149" s="54"/>
-    </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B150" s="31"/>
-      <c r="C150" s="33"/>
-      <c r="D150" s="33"/>
+      <c r="G149" s="33"/>
+      <c r="H149" s="34"/>
+    </row>
+    <row r="150" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B150" s="54"/>
+      <c r="C150" s="52"/>
+      <c r="D150" s="52"/>
       <c r="E150" s="15"/>
-      <c r="F150" s="28"/>
-      <c r="G150" s="55"/>
-      <c r="H150" s="56"/>
-    </row>
-    <row r="151" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="30" t="s">
+      <c r="F150" s="57"/>
+      <c r="G150" s="35"/>
+      <c r="H150" s="36"/>
+    </row>
+    <row r="151" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B151" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C151" s="32"/>
-      <c r="D151" s="33"/>
+      <c r="C151" s="55"/>
+      <c r="D151" s="52"/>
       <c r="E151" s="15"/>
-      <c r="F151" s="27" t="s">
+      <c r="F151" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="G151" s="49"/>
-      <c r="H151" s="50"/>
-    </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B152" s="31"/>
-      <c r="C152" s="33"/>
-      <c r="D152" s="33"/>
+      <c r="G151" s="29"/>
+      <c r="H151" s="30"/>
+    </row>
+    <row r="152" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B152" s="54"/>
+      <c r="C152" s="52"/>
+      <c r="D152" s="52"/>
       <c r="E152" s="15"/>
-      <c r="F152" s="29"/>
-      <c r="G152" s="51"/>
-      <c r="H152" s="52"/>
-    </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B153" s="30" t="s">
+      <c r="F152" s="58"/>
+      <c r="G152" s="31"/>
+      <c r="H152" s="32"/>
+    </row>
+    <row r="153" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B153" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C153" s="32"/>
-      <c r="D153" s="33"/>
+      <c r="C153" s="55"/>
+      <c r="D153" s="52"/>
       <c r="E153" s="15"/>
-      <c r="F153" s="27" t="s">
+      <c r="F153" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="G153" s="53"/>
-      <c r="H153" s="54"/>
-    </row>
-    <row r="154" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="31"/>
-      <c r="C154" s="33"/>
-      <c r="D154" s="33"/>
-      <c r="F154" s="28"/>
-      <c r="G154" s="55"/>
-      <c r="H154" s="56"/>
-    </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F155" s="27" t="s">
+      <c r="G153" s="33"/>
+      <c r="H153" s="34"/>
+    </row>
+    <row r="154" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="54"/>
+      <c r="C154" s="52"/>
+      <c r="D154" s="52"/>
+      <c r="F154" s="57"/>
+      <c r="G154" s="35"/>
+      <c r="H154" s="36"/>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F155" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="G155" s="49"/>
-      <c r="H155" s="50"/>
-    </row>
-    <row r="156" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F156" s="28"/>
-      <c r="G156" s="51"/>
-      <c r="H156" s="52"/>
-    </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F157" s="27" t="s">
+      <c r="G155" s="29"/>
+      <c r="H155" s="30"/>
+    </row>
+    <row r="156" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F156" s="57"/>
+      <c r="G156" s="31"/>
+      <c r="H156" s="32"/>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F157" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G157" s="49"/>
-      <c r="H157" s="50"/>
-    </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F158" s="28"/>
-      <c r="G158" s="51"/>
-      <c r="H158" s="52"/>
+      <c r="G157" s="29"/>
+      <c r="H157" s="30"/>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F158" s="57"/>
+      <c r="G158" s="31"/>
+      <c r="H158" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="G157:H158"/>
-    <mergeCell ref="G155:H156"/>
-    <mergeCell ref="G151:H152"/>
-    <mergeCell ref="G149:H150"/>
-    <mergeCell ref="G153:H154"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="F155:F156"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="C149:D150"/>
+    <mergeCell ref="C151:D152"/>
+    <mergeCell ref="C153:D154"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="C23:C29"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="D70:G70"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
@@ -2656,53 +2697,55 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="C42:C48"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="D68:G68"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="C23:C29"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="C149:D150"/>
-    <mergeCell ref="C151:D152"/>
-    <mergeCell ref="C153:D154"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="F155:F156"/>
+    <mergeCell ref="G157:H158"/>
+    <mergeCell ref="G155:H156"/>
+    <mergeCell ref="G151:H152"/>
+    <mergeCell ref="G149:H150"/>
+    <mergeCell ref="G153:H154"/>
   </mergeCells>
   <conditionalFormatting sqref="F23:F28">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>MOD(F23, 1) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:F38">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>MOD(F33, 1) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:F47">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>MOD(F42, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>MOD(F29, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>MOD(F39, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>MOD(F48, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>MOD(F54, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>MOD(F52, 1) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(F42, 1) = 0</formula>
+      <formula>MOD(F50, 1) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>